<commit_message>
Mark That Pawn 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Mlie/Mark That Pawn - 3056996662/Mark That Pawn - 3056996662.xlsx
+++ b/Data/Mlie/Mark That Pawn - 3056996662/Mark That Pawn - 3056996662.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Mark That Pawn - 3056996662\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FF4875-71F5-4A83-8F05-7C96C54508E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328D7BEF-497F-4BE3-8B3C-C4D883E31091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="703">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -2103,6 +2103,103 @@
   </si>
   <si>
     <t>폰의 사상 아이콘 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTP.OnlyWhenDraftedTT 'Will only apply when pawns are drafted' (English file: Text.xml:62)</t>
+  </si>
+  <si>
+    <t>MTP.OrLogic 'Or-logic' (English file: Text.xml:63)</t>
+  </si>
+  <si>
+    <t>MTP.OrLogicTT 'Will apply the rule if any of the selected things are correct, instead of when all are correct.' (English file: Text.xml:64)</t>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.TDFindLib 'Advanced rule (TD Find Lib)' (English file: Text.xml:141)</t>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.Mechanoid 'Specific mechanoid' (English file: Text.xml:142)</t>
+  </si>
+  <si>
+    <t>MTP.TDFindLibRuleLabel 'Mark That Pawn-rule' (English file: Text.xml:143)</t>
+  </si>
+  <si>
+    <t>MTP.RequiresAnActiveGame 'Requires an active game' (English file: Text.xml:144)</t>
+  </si>
+  <si>
+    <t>MTP.EditTdRule 'Edit' (English file: Text.xml:145)</t>
+  </si>
+  <si>
+    <t>MTP.OnlyWhenDraftedTT</t>
+  </si>
+  <si>
+    <t>MTP.OrLogicTT</t>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.TDFindLib</t>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.Mechanoid</t>
+  </si>
+  <si>
+    <t>MTP.TDFindLibRuleLabel</t>
+  </si>
+  <si>
+    <t>MTP.RequiresAnActiveGame</t>
+  </si>
+  <si>
+    <t>MTP.EditTdRule</t>
+  </si>
+  <si>
+    <t>MTP.OrLogic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Will only apply when pawns are drafted</t>
+  </si>
+  <si>
+    <t>Or-logic</t>
+  </si>
+  <si>
+    <t>Will apply the rule if any of the selected things are correct, instead of when all are correct.</t>
+  </si>
+  <si>
+    <t>Advanced rule (TD Find Lib)</t>
+  </si>
+  <si>
+    <t>Specific mechanoid</t>
+  </si>
+  <si>
+    <t>Mark That Pawn-rule</t>
+  </si>
+  <si>
+    <t>Requires an active game</t>
+  </si>
+  <si>
+    <t>폰을 소집할 때만 적용됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Or-논리</t>
+  </si>
+  <si>
+    <t>모든 항목이 맞을 때가 아니라 선택한 항목 중 하나라도 맞으면 규칙을 적용합니다.</t>
+  </si>
+  <si>
+    <t>고급 규칙(TD Find Lib)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특정 메카노이드</t>
+  </si>
+  <si>
+    <t>Mark That Pawn-규칙</t>
+  </si>
+  <si>
+    <t>게임이 활성화되어 있어야 합니다.</t>
+  </si>
+  <si>
+    <t>Edit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2476,10 +2573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G167"/>
+  <dimension ref="A1:H175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5227,7 +5324,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>648</v>
       </c>
@@ -5244,7 +5341,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>650</v>
       </c>
@@ -5261,7 +5358,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>652</v>
       </c>
@@ -5278,7 +5375,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>654</v>
       </c>
@@ -5295,7 +5392,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>656</v>
       </c>
@@ -5312,7 +5409,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>657</v>
       </c>
@@ -5329,7 +5426,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>659</v>
       </c>
@@ -5344,6 +5441,206 @@
       </c>
       <c r="E167" t="s">
         <v>671</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B168" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C168" t="s">
+        <v>680</v>
+      </c>
+      <c r="D168" t="s">
+        <v>688</v>
+      </c>
+      <c r="E168" t="s">
+        <v>695</v>
+      </c>
+      <c r="F168" t="s">
+        <v>672</v>
+      </c>
+      <c r="G168" t="str">
+        <f>LEFT(F168,FIND(" ",F168)-1)</f>
+        <v>MTP.OnlyWhenDraftedTT</v>
+      </c>
+      <c r="H168" t="str">
+        <f>MID(F168,FIND("'",F168)+1,FIND("'",F168,FIND("'",F168)+1)-FIND("'",F168)-1)</f>
+        <v>Will only apply when pawns are drafted</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B169" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C169" t="s">
+        <v>687</v>
+      </c>
+      <c r="D169" t="s">
+        <v>689</v>
+      </c>
+      <c r="E169" t="s">
+        <v>696</v>
+      </c>
+      <c r="F169" t="s">
+        <v>673</v>
+      </c>
+      <c r="G169" t="str">
+        <f t="shared" ref="G169:G175" si="0">LEFT(F169,FIND(" ",F169)-1)</f>
+        <v>MTP.OrLogic</v>
+      </c>
+      <c r="H169" t="str">
+        <f t="shared" ref="H169:H175" si="1">MID(F169,FIND("'",F169)+1,FIND("'",F169,FIND("'",F169)+1)-FIND("'",F169)-1)</f>
+        <v>Or-logic</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B170" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C170" t="s">
+        <v>681</v>
+      </c>
+      <c r="D170" t="s">
+        <v>690</v>
+      </c>
+      <c r="E170" t="s">
+        <v>697</v>
+      </c>
+      <c r="F170" t="s">
+        <v>674</v>
+      </c>
+      <c r="G170" t="str">
+        <f t="shared" si="0"/>
+        <v>MTP.OrLogicTT</v>
+      </c>
+      <c r="H170" t="str">
+        <f t="shared" si="1"/>
+        <v>Will apply the rule if any of the selected things are correct, instead of when all are correct.</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B171" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C171" t="s">
+        <v>682</v>
+      </c>
+      <c r="D171" t="s">
+        <v>691</v>
+      </c>
+      <c r="E171" t="s">
+        <v>698</v>
+      </c>
+      <c r="F171" t="s">
+        <v>675</v>
+      </c>
+      <c r="G171" t="str">
+        <f t="shared" si="0"/>
+        <v>MTP.AutomaticType.TDFindLib</v>
+      </c>
+      <c r="H171" t="str">
+        <f t="shared" si="1"/>
+        <v>Advanced rule (TD Find Lib)</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B172" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C172" t="s">
+        <v>683</v>
+      </c>
+      <c r="D172" t="s">
+        <v>692</v>
+      </c>
+      <c r="E172" t="s">
+        <v>699</v>
+      </c>
+      <c r="F172" t="s">
+        <v>676</v>
+      </c>
+      <c r="G172" t="str">
+        <f t="shared" si="0"/>
+        <v>MTP.AutomaticType.Mechanoid</v>
+      </c>
+      <c r="H172" t="str">
+        <f t="shared" si="1"/>
+        <v>Specific mechanoid</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B173" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C173" t="s">
+        <v>684</v>
+      </c>
+      <c r="D173" t="s">
+        <v>693</v>
+      </c>
+      <c r="E173" t="s">
+        <v>700</v>
+      </c>
+      <c r="F173" t="s">
+        <v>677</v>
+      </c>
+      <c r="G173" t="str">
+        <f t="shared" si="0"/>
+        <v>MTP.TDFindLibRuleLabel</v>
+      </c>
+      <c r="H173" t="str">
+        <f t="shared" si="1"/>
+        <v>Mark That Pawn-rule</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B174" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C174" t="s">
+        <v>685</v>
+      </c>
+      <c r="D174" t="s">
+        <v>694</v>
+      </c>
+      <c r="E174" t="s">
+        <v>701</v>
+      </c>
+      <c r="F174" t="s">
+        <v>678</v>
+      </c>
+      <c r="G174" t="str">
+        <f t="shared" si="0"/>
+        <v>MTP.RequiresAnActiveGame</v>
+      </c>
+      <c r="H174" t="str">
+        <f t="shared" si="1"/>
+        <v>Requires an active game</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B175" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C175" t="s">
+        <v>686</v>
+      </c>
+      <c r="D175" t="s">
+        <v>702</v>
+      </c>
+      <c r="E175" t="s">
+        <v>540</v>
+      </c>
+      <c r="F175" t="s">
+        <v>679</v>
+      </c>
+      <c r="G175" t="str">
+        <f t="shared" si="0"/>
+        <v>MTP.EditTdRule</v>
+      </c>
+      <c r="H175" t="str">
+        <f t="shared" si="1"/>
+        <v>Edit</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mark That Pawn - 3056996662 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Mlie/Mark That Pawn - 3056996662/Mark That Pawn - 3056996662.xlsx
+++ b/Data/Mlie/Mark That Pawn - 3056996662/Mark That Pawn - 3056996662.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Mark That Pawn - 3056996662\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328D7BEF-497F-4BE3-8B3C-C4D883E31091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E277E3AF-F512-499C-8AAB-1C89CBB2F458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="711">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -2201,6 +2201,30 @@
   <si>
     <t>Edit</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.FactionLeader</t>
+  </si>
+  <si>
+    <t>MTP.RequiresASpecificGame</t>
+  </si>
+  <si>
+    <t>MTP.IsInWrongGame</t>
+  </si>
+  <si>
+    <t>Show faction leader</t>
+  </si>
+  <si>
+    <t>Created in another save</t>
+  </si>
+  <si>
+    <t>진영 지도자 표시</t>
+  </si>
+  <si>
+    <t>활성화된 게임이 필요합니다.</t>
+  </si>
+  <si>
+    <t>다른 저장에서 생성</t>
   </si>
 </sst>
 </file>
@@ -2573,10 +2597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E176" sqref="E176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5643,6 +5667,48 @@
         <v>Edit</v>
       </c>
     </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B176" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C176" t="s">
+        <v>703</v>
+      </c>
+      <c r="D176" t="s">
+        <v>706</v>
+      </c>
+      <c r="E176" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B177" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C177" t="s">
+        <v>704</v>
+      </c>
+      <c r="D177" t="s">
+        <v>694</v>
+      </c>
+      <c r="E177" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B178" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C178" t="s">
+        <v>705</v>
+      </c>
+      <c r="D178" t="s">
+        <v>707</v>
+      </c>
+      <c r="E178" t="s">
+        <v>710</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>